<commit_message>
More work on storing and retrieving serialized data
</commit_message>
<xml_diff>
--- a/JobData.xlsx
+++ b/JobData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macke\Documents\Otech\PROG2002\JobApplicationTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F2494C-BC6B-4821-9C29-F53300CB0107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCB036C-3708-47F5-B5E8-50CE7D48A0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="JobList" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>

</xml_diff>